<commit_message>
Ausreißer (05.05.) aus dem Rohdatensatz df entfernt; Jahreszeitenvariablen (Fruehling, Sommer, Herbst, WInter) angelegt; erste Ansätze naives Modell Vorwochenwert
</commit_message>
<xml_diff>
--- a/data/TdDE.xlsx
+++ b/data/TdDE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solsken\Documents\Studium\FH Kiel\SS2020\Projekt_SoSe2020\Application_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99957798-3948-4A10-8629-62AF11DFEA98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745305AE-19C6-4577-9C1D-785EF327261E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="888" windowWidth="17280" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
   <dimension ref="A1:B244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>